<commit_message>
15022021 -modificacion a reporte solicitado desde gestion personas. -modificacion a excel para reporte
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/FueraPlazo.xlsx
+++ b/App.Web/App_Data/FueraPlazo.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\Reportes\Cometidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GestionProcesos\SourceNew\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cometido Fuera de Plazo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cometido Fuera de Plazo'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Unidad de desempeño</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Cantidad de días</t>
+  </si>
+  <si>
+    <t>Fecha Inicio</t>
   </si>
 </sst>
 </file>
@@ -372,10 +375,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,7 +390,7 @@
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,6 +403,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>

</xml_diff>